<commit_message>
Updates to code to reflect Paul and Hilary's comments.
Min/resp removed from sedimentation function.

Hilary and Paul's mineralization routine added.

POC aerial and POC inflow split apart in SWGW function in order to track POC sourcing.
</commit_message>
<xml_diff>
--- a/TroutLake/ParameterInputsTrout.xlsx
+++ b/TroutLake/ParameterInputsTrout.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>LakePerimeter</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>#SWGW Parameters</t>
+  </si>
+  <si>
+    <t>#Min/Resp Parameters</t>
+  </si>
+  <si>
+    <t>DOC_miner_const</t>
   </si>
 </sst>
 </file>
@@ -431,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,6 +640,22 @@
         <v>22</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
NPP function and related variables changed to GPP to reflect what they actually area.
Split of GPP contributions to DOC and POC added per Mindy's input.

Aerial and wetland loading algorithms changed to reflect per day rate constant, instead of per year rate constant.

Respiration algorithm added. Respiration algorithm is currently crashing the DOC concentration.
</commit_message>
<xml_diff>
--- a/TroutLake/ParameterInputsTrout.xlsx
+++ b/TroutLake/ParameterInputsTrout.xlsx
@@ -101,12 +101,6 @@
     <t>Parameter</t>
   </si>
   <si>
-    <t>gPOC/m/yr</t>
-  </si>
-  <si>
-    <t>gDOC/m/yr</t>
-  </si>
-  <si>
     <t>#General Parameters</t>
   </si>
   <si>
@@ -120,6 +114,12 @@
   </si>
   <si>
     <t>DOC_miner_const</t>
+  </si>
+  <si>
+    <t>gPOC/m/d</t>
+  </si>
+  <si>
+    <t>gDOC/m/d</t>
   </si>
 </sst>
 </file>
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +462,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -533,7 +533,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -549,7 +549,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -582,7 +582,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -593,7 +593,7 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -642,12 +642,12 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B21">
         <v>5.0000000000000001E-3</v>

</xml_diff>

<commit_message>
update to mineralization parameter
</commit_message>
<xml_diff>
--- a/TroutLake/ParameterInputsTrout.xlsx
+++ b/TroutLake/ParameterInputsTrout.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek\Box Sync\GLEON\SOS\TroutLake\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15720" windowHeight="5925"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -429,7 +424,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -440,7 +435,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,7 +645,7 @@
         <v>29</v>
       </c>
       <c r="B21">
-        <v>5.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Update to respiration routine. Change of name for GPP to NPP to reflect calculations. Added parameteter for updated Resp routine. General housekeeping.
</commit_message>
<xml_diff>
--- a/TroutLake/ParameterInputsTrout.xlsx
+++ b/TroutLake/ParameterInputsTrout.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek\Box Sync\GLEON\SOS\TroutLake\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15720" windowHeight="5925"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>LakePerimeter</t>
   </si>
@@ -115,6 +120,9 @@
   </si>
   <si>
     <t>gDOC/m/d</t>
+  </si>
+  <si>
+    <t>RespParam</t>
   </si>
 </sst>
 </file>
@@ -424,7 +432,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -432,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,6 +659,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22">
+        <v>1E-3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update prop_Gw inflow to 0.19
</commit_message>
<xml_diff>
--- a/TroutLake/ParameterInputsTrout.xlsx
+++ b/TroutLake/ParameterInputsTrout.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek\Box Sync\GLEON\SOS\TroutLake\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15720" windowHeight="5925"/>
   </bookViews>
@@ -432,7 +427,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -442,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +599,7 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>0.19</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Time-series file headers updated. Parameter file updated. Code changes reflect changes in time-series header.
</commit_message>
<xml_diff>
--- a/TroutLake/ParameterInputsTrout.xlsx
+++ b/TroutLake/ParameterInputsTrout.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>LakePerimeter</t>
   </si>
@@ -81,43 +81,40 @@
     <t>PropGW</t>
   </si>
   <si>
+    <t>g/m3</t>
+  </si>
+  <si>
+    <t>DOC_precip</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>#General Parameters</t>
+  </si>
+  <si>
+    <t>#Sedimentation Parameters</t>
+  </si>
+  <si>
+    <t>#SWGW Parameters</t>
+  </si>
+  <si>
+    <t>#Min/Resp Parameters</t>
+  </si>
+  <si>
+    <t>DOC_miner_const</t>
+  </si>
+  <si>
+    <t>gPOC/m/d</t>
+  </si>
+  <si>
+    <t>gDOC/m/d</t>
+  </si>
+  <si>
+    <t>RespParam</t>
+  </si>
+  <si>
     <t>DOC_gw</t>
-  </si>
-  <si>
-    <t>DOC_sw</t>
-  </si>
-  <si>
-    <t>g/m3</t>
-  </si>
-  <si>
-    <t>DOC_precip</t>
-  </si>
-  <si>
-    <t>Parameter</t>
-  </si>
-  <si>
-    <t>#General Parameters</t>
-  </si>
-  <si>
-    <t>#Sedimentation Parameters</t>
-  </si>
-  <si>
-    <t>#SWGW Parameters</t>
-  </si>
-  <si>
-    <t>#Min/Resp Parameters</t>
-  </si>
-  <si>
-    <t>DOC_miner_const</t>
-  </si>
-  <si>
-    <t>gPOC/m/d</t>
-  </si>
-  <si>
-    <t>gDOC/m/d</t>
-  </si>
-  <si>
-    <t>RespParam</t>
   </si>
 </sst>
 </file>
@@ -438,7 +435,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +446,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -460,7 +457,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -531,7 +528,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -547,7 +544,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -580,7 +577,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -591,61 +588,50 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B16">
-        <v>0.19</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
-        <v>10</v>
+        <v>0.19</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18">
-        <v>5.8</v>
-      </c>
-      <c r="C18" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B21">
         <v>3.0000000000000001E-3</v>
@@ -656,7 +642,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B22">
         <v>1E-3</v>

</xml_diff>

<commit_message>
Expand time series, complete data seeking for time series, update Comments & Quirks file of data sources
</commit_message>
<xml_diff>
--- a/TroutLake/ParameterInputsTrout.xlsx
+++ b/TroutLake/ParameterInputsTrout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15720" windowHeight="5925"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="15720" windowHeight="5865"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -150,8 +150,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,7 +425,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -435,12 +436,13 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -465,7 +467,7 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>32448</v>
+        <v>25900</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -487,7 +489,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>15650000</v>
+        <v>16079000</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -497,8 +499,9 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
-        <v>229000000</v>
+      <c r="B6" s="1">
+        <f>B4*B5</f>
+        <v>234753400</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -613,14 +616,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="B19">
+      <c r="B18">
         <v>2</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C18" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>